<commit_message>
Attempted to fix naming and formatting shortcumings, but failed. Made changes elsewhere, however.
</commit_message>
<xml_diff>
--- a/upl_file_bunker/2425_Report.xlsx
+++ b/upl_file_bunker/2425_Report.xlsx
@@ -7314,7 +7314,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Latin American, CARIBBEAN, And Latino Studies, M.A.</t>
+          <t>Latin American, CARIBBEAN, and latino studies,  m.a.</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -12142,7 +12142,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Women'S, GENDER, And Sexuality Studies, M.A.</t>
+          <t>Women'S, GENDER, and sexuality studies,  m.a.</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -14386,7 +14386,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>Compliance, RISK, &amp; Anti-Money Laundering Graduate Certificate</t>
+          <t>Compliance, RISK, &amp; anti-money laundering graduate certificate</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
@@ -18806,7 +18806,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>Pharmacy Entrepreneurship, LEADERSHIP &amp; Management Graduate Certificate</t>
+          <t>Pharmacy Entrepreneurship, LEADERSHIP &amp; management graduate certificate</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
@@ -19622,7 +19622,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>Scholarly Excellence, LEADERSHIP Experiences, &amp; Collaborative Training (S.E.L.E.C.T) Graduate Certificate</t>
+          <t>Scholarly Excellence, LEADERSHIP experiences,  &amp; collaborative training (s.e.l.e.c.t) graduate certificate</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -21050,7 +21050,7 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>Water, HEALTH And Sustainability Graduate Certificate</t>
+          <t>Water, HEALTH and sustainability graduate certificate</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
@@ -21186,7 +21186,7 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>Women'S, GENDER, And Sexuality Studies Graduate Certificate</t>
+          <t>Women'S, GENDER, and sexuality studies graduate certificate</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
@@ -21798,7 +21798,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>Language, SPEECH, And Hearing Sciences B.A.</t>
+          <t>Language, SPEECH, and hearing sciences b.a.</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
@@ -22002,7 +22002,7 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>Criminology B.A., WITH Cybercrime Concentration</t>
+          <t>Criminology B.A., WITH cybercrime concentration</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
@@ -22138,7 +22138,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>Behavioral Healthcare B.S., WITH Applied Behavior Analysis Concentration</t>
+          <t>Behavioral Healthcare B.S., WITH applied behavior analysis concentration</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
@@ -22206,7 +22206,7 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>Behavioral Healthcare B.S., WITH Behavioral Health Across The Lifespan Concentration</t>
+          <t>Behavioral Healthcare B.S., WITH behavioral health across the lifespan concentration</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
@@ -22274,7 +22274,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>Behavioral Healthcare B.S., WITH Children'S Behavioral Healthcare Concentration</t>
+          <t>Behavioral Healthcare B.S., WITH children's behavioral healthcare concentration</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
@@ -23022,7 +23022,7 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>Mathematics Education B.S., WITH Middle School Mathematics Concentration</t>
+          <t>Mathematics Education B.S., WITH middle school mathematics concentration</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
@@ -23090,7 +23090,7 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>Science Education B.S., WITH Biology Education Concentration</t>
+          <t>Science Education B.S., WITH biology education concentration</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
@@ -23158,7 +23158,7 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>Science Education B.S., WITH Chemistry Education Concentration</t>
+          <t>Science Education B.S., WITH chemistry education concentration</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
@@ -23226,7 +23226,7 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>Science Education B.S., WITH Physics Education Concentration</t>
+          <t>Science Education B.S., WITH physics education concentration</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
@@ -25264,7 +25264,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>Health Sciences B.S., WITH Aging Health Studies And Health Care Administration Concentration</t>
+          <t>Health Sciences B.S., WITH aging health studies and health care administration concentration</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
@@ -25332,7 +25332,7 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>Health Sciences B.S., WITH Aging Health Studies And Health Information Technology Concentration</t>
+          <t>Health Sciences B.S., WITH aging health studies and health information technology concentration</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
@@ -25400,7 +25400,7 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>Health Sciences B.S., WITH Aging Health Studies Concentration</t>
+          <t>Health Sciences B.S., WITH aging health studies concentration</t>
         </is>
       </c>
       <c r="B368" t="inlineStr">
@@ -25468,7 +25468,7 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>Health Sciences B.S., WITH Biological Health Sciences And Aging Health Studies Concentration</t>
+          <t>Health Sciences B.S., WITH biological health sciences and aging health studies concentration</t>
         </is>
       </c>
       <c r="B369" t="inlineStr">
@@ -25536,7 +25536,7 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>Health Sciences B.S., WITH Biological Health Sciences And Health Care Administration Concentration</t>
+          <t>Health Sciences B.S., WITH biological health sciences and health care administration concentration</t>
         </is>
       </c>
       <c r="B370" t="inlineStr">
@@ -25604,7 +25604,7 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>Health Sciences B.S., WITH Biological Health Sciences And Health Information Technology Concentration</t>
+          <t>Health Sciences B.S., WITH biological health sciences and health information technology concentration</t>
         </is>
       </c>
       <c r="B371" t="inlineStr">
@@ -25672,7 +25672,7 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>Health Sciences B.S., WITH Biological Health Sciences And Social And Behavioral Health Sciences Concentration</t>
+          <t>Health Sciences B.S., WITH biological health sciences and social and behavioral health sciences concentration</t>
         </is>
       </c>
       <c r="B372" t="inlineStr">
@@ -25740,7 +25740,7 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>Health Sciences B.S., WITH Biological Health Sciences Concentration</t>
+          <t>Health Sciences B.S., WITH biological health sciences concentration</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
@@ -25808,7 +25808,7 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>Health Sciences B.S., WITH Health Care Administration And Health Information Technology Concentration</t>
+          <t>Health Sciences B.S., WITH health care administration and health information technology concentration</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
@@ -25876,7 +25876,7 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>Health Sciences B.S., WITH Health Care Administration Concentration</t>
+          <t>Health Sciences B.S., WITH health care administration concentration</t>
         </is>
       </c>
       <c r="B375" t="inlineStr">
@@ -25944,7 +25944,7 @@
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>Health Sciences B.S., WITH Health Information Technology Concentration</t>
+          <t>Health Sciences B.S., WITH health information technology concentration</t>
         </is>
       </c>
       <c r="B376" t="inlineStr">
@@ -26012,7 +26012,7 @@
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>Health Sciences B.S., WITH Nutrition Science Concentration</t>
+          <t>Health Sciences B.S., WITH nutrition science concentration</t>
         </is>
       </c>
       <c r="B377" t="inlineStr">
@@ -26080,7 +26080,7 @@
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>Health Sciences B.S., WITH Social And Behavioral Health Sciences And Aging Health Studies Concentration</t>
+          <t>Health Sciences B.S., WITH social and behavioral health sciences and aging health studies concentration</t>
         </is>
       </c>
       <c r="B378" t="inlineStr">
@@ -26148,7 +26148,7 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>Health Sciences B.S., WITH Social And Behavioral Health Sciences And Health Care Administration Concentration</t>
+          <t>Health Sciences B.S., WITH social and behavioral health sciences and health care administration concentration</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
@@ -26216,7 +26216,7 @@
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>Health Sciences B.S., WITH Social And Behavioral Health Sciences And Health Information Technology Concentration</t>
+          <t>Health Sciences B.S., WITH social and behavioral health sciences and health information technology concentration</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
@@ -26284,7 +26284,7 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>Health Sciences B.S., WITH Social And Behavioral Health Sciences Concentration</t>
+          <t>Health Sciences B.S., WITH social and behavioral health sciences concentration</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
@@ -26828,7 +26828,7 @@
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>Graphic Arts B.F.A, WITH Graphic Design Concentration</t>
+          <t>Graphic Arts B.F.A, WITH graphic design concentration</t>
         </is>
       </c>
       <c r="B389" t="inlineStr">
@@ -26896,7 +26896,7 @@
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>Graphic Arts B.F.A, WITH Illustration Concentration</t>
+          <t>Graphic Arts B.F.A, WITH illustration concentration</t>
         </is>
       </c>
       <c r="B390" t="inlineStr">
@@ -27032,7 +27032,7 @@
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>Studio Art B.F.A., WITH Animation And Digital Modeling Concentration</t>
+          <t>Studio Art B.F.A., WITH animation and digital modeling concentration</t>
         </is>
       </c>
       <c r="B392" t="inlineStr">
@@ -27438,7 +27438,7 @@
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>Music Performance B.M., WITH Acoustic &amp; Electronic Composition Concentration</t>
+          <t>Music Performance B.M., WITH acoustic &amp; electronic composition concentration</t>
         </is>
       </c>
       <c r="B398" t="inlineStr">
@@ -27506,7 +27506,7 @@
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>Music Performance B.M., WITH Contemporary Commercial Music Concentration</t>
+          <t>Music Performance B.M., WITH contemporary commercial music concentration</t>
         </is>
       </c>
       <c r="B399" t="inlineStr">
@@ -27574,7 +27574,7 @@
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>Music Performance B.M., WITH Jazz Studies Concentration</t>
+          <t>Music Performance B.M., WITH jazz studies concentration</t>
         </is>
       </c>
       <c r="B400" t="inlineStr">
@@ -27642,7 +27642,7 @@
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>Music Performance B.M., WITH Performance Concentration</t>
+          <t>Music Performance B.M., WITH performance concentration</t>
         </is>
       </c>
       <c r="B401" t="inlineStr">
@@ -27710,7 +27710,7 @@
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>Dance B.A., WITH Dance Studies Concentration</t>
+          <t>Dance B.A., WITH dance studies concentration</t>
         </is>
       </c>
       <c r="B402" t="inlineStr">
@@ -27778,7 +27778,7 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>Dance B.F.A., WITH Ballet Concentration</t>
+          <t>Dance B.F.A., WITH ballet concentration</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
@@ -27846,7 +27846,7 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>Dance B.F.A., WITH Modern Dance Concentration</t>
+          <t>Dance B.F.A., WITH modern dance concentration</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
@@ -27982,7 +27982,7 @@
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>Theatre B.A., WITH Design And Technology Concentration</t>
+          <t>Theatre B.A., WITH design and technology concentration</t>
         </is>
       </c>
       <c r="B406" t="inlineStr">
@@ -28050,7 +28050,7 @@
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>Theatre B.A., WITH Performance Concentration</t>
+          <t>Theatre B.A., WITH performance concentration</t>
         </is>
       </c>
       <c r="B407" t="inlineStr">
@@ -28118,7 +28118,7 @@
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>Theatre B.A., WITH Theatre Arts Concentration</t>
+          <t>Theatre B.A., WITH theatre arts concentration</t>
         </is>
       </c>
       <c r="B408" t="inlineStr">
@@ -28730,7 +28730,7 @@
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>Finance B.S., WITH Corporate Finance Concentration</t>
+          <t>Finance B.S., WITH corporate finance concentration</t>
         </is>
       </c>
       <c r="B417" t="inlineStr">
@@ -28798,7 +28798,7 @@
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>Finance B.S., WITH Fintech Concentration</t>
+          <t>Finance B.S., WITH fintech concentration</t>
         </is>
       </c>
       <c r="B418" t="inlineStr">
@@ -28866,7 +28866,7 @@
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>Finance B.S., WITH Investment Analysis Concentration</t>
+          <t>Finance B.S., WITH investment analysis concentration</t>
         </is>
       </c>
       <c r="B419" t="inlineStr">
@@ -28934,7 +28934,7 @@
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t>Finance B.S., WITH Real Estate Concentration</t>
+          <t>Finance B.S., WITH real estate concentration</t>
         </is>
       </c>
       <c r="B420" t="inlineStr">
@@ -29750,7 +29750,7 @@
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>Business Analytics And Information Systems B.S., WITH Cybersecurity Concentration</t>
+          <t>Business Analytics And Information Systems B.S., WITH cybersecurity concentration</t>
         </is>
       </c>
       <c r="B432" t="inlineStr">
@@ -29954,7 +29954,7 @@
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>Management B.S., WITH Aging Services Management Concentration</t>
+          <t>Management B.S., WITH aging services management concentration</t>
         </is>
       </c>
       <c r="B435" t="inlineStr">
@@ -30022,7 +30022,7 @@
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>Management B.S., WITH Human Resources Management Concentration</t>
+          <t>Management B.S., WITH human resources management concentration</t>
         </is>
       </c>
       <c r="B436" t="inlineStr">
@@ -30090,7 +30090,7 @@
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t>Management B.S., WITH Project Management Concentration</t>
+          <t>Management B.S., WITH project management concentration</t>
         </is>
       </c>
       <c r="B437" t="inlineStr">
@@ -30566,7 +30566,7 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>Global Business B.A., WITH Business Analytics And Information Systems Concentration</t>
+          <t>Global Business B.A., WITH business analytics and information systems concentration</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
@@ -30634,7 +30634,7 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>Global Business B.A., WITH Finance Concentration</t>
+          <t>Global Business B.A., WITH finance concentration</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
@@ -30702,7 +30702,7 @@
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>Global Business B.A., WITH Management Concentration</t>
+          <t>Global Business B.A., WITH management concentration</t>
         </is>
       </c>
       <c r="B446" t="inlineStr">
@@ -30770,7 +30770,7 @@
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>Global Business B.A., WITH Marketing Concentration</t>
+          <t>Global Business B.A., WITH marketing concentration</t>
         </is>
       </c>
       <c r="B447" t="inlineStr">
@@ -30906,7 +30906,7 @@
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t>Marketing B.S., WITH Digital Marketing Concentration</t>
+          <t>Marketing B.S., WITH digital marketing concentration</t>
         </is>
       </c>
       <c r="B449" t="inlineStr">
@@ -30974,7 +30974,7 @@
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>Marketing B.S., WITH Entrepreneurship Concentration</t>
+          <t>Marketing B.S., WITH entrepreneurship concentration</t>
         </is>
       </c>
       <c r="B450" t="inlineStr">
@@ -31042,7 +31042,7 @@
     <row r="451">
       <c r="A451" t="inlineStr">
         <is>
-          <t>Marketing B.S., WITH Sales Concentration</t>
+          <t>Marketing B.S., WITH sales concentration</t>
         </is>
       </c>
       <c r="B451" t="inlineStr">
@@ -31110,7 +31110,7 @@
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>Marketing B.S., WITH Sport And Entertainment Management Concentration</t>
+          <t>Marketing B.S., WITH sport and entertainment management concentration</t>
         </is>
       </c>
       <c r="B452" t="inlineStr">
@@ -31926,7 +31926,7 @@
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>Applied Science B.S.A.S., WITH Aging Sciences Concentration</t>
+          <t>Applied Science B.S.A.S., WITH aging sciences concentration</t>
         </is>
       </c>
       <c r="B464" t="inlineStr">
@@ -31994,7 +31994,7 @@
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t>Applied Science B.S.A.S., WITH Applied Behavior Analysis Concentration</t>
+          <t>Applied Science B.S.A.S., WITH applied behavior analysis concentration</t>
         </is>
       </c>
       <c r="B465" t="inlineStr">
@@ -32062,7 +32062,7 @@
     <row r="466">
       <c r="A466" t="inlineStr">
         <is>
-          <t>Applied Science B.S.A.S., WITH Behavioral Healthcare Concentration</t>
+          <t>Applied Science B.S.A.S., WITH behavioral healthcare concentration</t>
         </is>
       </c>
       <c r="B466" t="inlineStr">
@@ -32130,7 +32130,7 @@
     <row r="467">
       <c r="A467" t="inlineStr">
         <is>
-          <t>Applied Science B.S.A.S., WITH Criminal Justice Concentration</t>
+          <t>Applied Science B.S.A.S., WITH criminal justice concentration</t>
         </is>
       </c>
       <c r="B467" t="inlineStr">
@@ -32198,7 +32198,7 @@
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>Applied Science B.S.A.S., WITH Environmental Policy Concentration</t>
+          <t>Applied Science B.S.A.S., WITH environmental policy concentration</t>
         </is>
       </c>
       <c r="B468" t="inlineStr">
@@ -32266,7 +32266,7 @@
     <row r="469">
       <c r="A469" t="inlineStr">
         <is>
-          <t>Applied Science B.S.A.S., WITH Hospitality Management Concentration</t>
+          <t>Applied Science B.S.A.S., WITH hospitality management concentration</t>
         </is>
       </c>
       <c r="B469" t="inlineStr">
@@ -32334,7 +32334,7 @@
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>Applied Science B.S.A.S., WITH Information Studies: Information Architecture Concentration</t>
+          <t>Applied Science B.S.A.S., WITH information studies: information architecture concentration</t>
         </is>
       </c>
       <c r="B470" t="inlineStr">
@@ -32402,7 +32402,7 @@
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>Applied Science B.S.A.S., WITH Leadership Studies Concentration</t>
+          <t>Applied Science B.S.A.S., WITH leadership studies concentration</t>
         </is>
       </c>
       <c r="B471" t="inlineStr">
@@ -32470,7 +32470,7 @@
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>Applied Science B.S.A.S., WITH Public Health Concentration</t>
+          <t>Applied Science B.S.A.S., WITH public health concentration</t>
         </is>
       </c>
       <c r="B472" t="inlineStr">
@@ -32538,7 +32538,7 @@
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>Applied Science B.S.A.S., WITH Public Service And Leadership Concentration</t>
+          <t>Applied Science B.S.A.S., WITH public service and leadership concentration</t>
         </is>
       </c>
       <c r="B473" t="inlineStr">
@@ -32606,7 +32606,7 @@
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t>Applied Science B.S.A.S., WITH Urban Studies Concentration</t>
+          <t>Applied Science B.S.A.S., WITH urban studies concentration</t>
         </is>
       </c>
       <c r="B474" t="inlineStr">
@@ -32674,7 +32674,7 @@
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t>General Studies B.G.S., WITH Applied Behavior Analysis Concentration</t>
+          <t>General Studies B.G.S., WITH applied behavior analysis concentration</t>
         </is>
       </c>
       <c r="B475" t="inlineStr">
@@ -32742,7 +32742,7 @@
     <row r="476">
       <c r="A476" t="inlineStr">
         <is>
-          <t>General Studies B.G.S., WITH Behavioral Healthcare Concentration</t>
+          <t>General Studies B.G.S., WITH behavioral healthcare concentration</t>
         </is>
       </c>
       <c r="B476" t="inlineStr">
@@ -32810,7 +32810,7 @@
     <row r="477">
       <c r="A477" t="inlineStr">
         <is>
-          <t>General Studies B.G.S., WITH Business Concentration</t>
+          <t>General Studies B.G.S., WITH business concentration</t>
         </is>
       </c>
       <c r="B477" t="inlineStr">
@@ -32878,7 +32878,7 @@
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>General Studies B.G.S., WITH Criminal Justice Concentration</t>
+          <t>General Studies B.G.S., WITH criminal justice concentration</t>
         </is>
       </c>
       <c r="B478" t="inlineStr">
@@ -32946,7 +32946,7 @@
     <row r="479">
       <c r="A479" t="inlineStr">
         <is>
-          <t>General Studies B.G.S., WITH Environmental Policy Concentration</t>
+          <t>General Studies B.G.S., WITH environmental policy concentration</t>
         </is>
       </c>
       <c r="B479" t="inlineStr">
@@ -33014,7 +33014,7 @@
     <row r="480">
       <c r="A480" t="inlineStr">
         <is>
-          <t>General Studies B.G.S., WITH Hospitality Management Concentration</t>
+          <t>General Studies B.G.S., WITH hospitality management concentration</t>
         </is>
       </c>
       <c r="B480" t="inlineStr">
@@ -33082,7 +33082,7 @@
     <row r="481">
       <c r="A481" t="inlineStr">
         <is>
-          <t>General Studies B.G.S., WITH Information Studies: Information Architecture Concentration</t>
+          <t>General Studies B.G.S., WITH information studies: information architecture concentration</t>
         </is>
       </c>
       <c r="B481" t="inlineStr">
@@ -33150,7 +33150,7 @@
     <row r="482">
       <c r="A482" t="inlineStr">
         <is>
-          <t>General Studies B.G.S., WITH Leadership Studies Concentration</t>
+          <t>General Studies B.G.S., WITH leadership studies concentration</t>
         </is>
       </c>
       <c r="B482" t="inlineStr">
@@ -33218,7 +33218,7 @@
     <row r="483">
       <c r="A483" t="inlineStr">
         <is>
-          <t>General Studies B.G.S., WITH Public Health Concentration</t>
+          <t>General Studies B.G.S., WITH public health concentration</t>
         </is>
       </c>
       <c r="B483" t="inlineStr">
@@ -33286,7 +33286,7 @@
     <row r="484">
       <c r="A484" t="inlineStr">
         <is>
-          <t>General Studies B.G.S., WITH Public Service And Leadership Concentration</t>
+          <t>General Studies B.G.S., WITH public service and leadership concentration</t>
         </is>
       </c>
       <c r="B484" t="inlineStr">
@@ -33354,7 +33354,7 @@
     <row r="485">
       <c r="A485" t="inlineStr">
         <is>
-          <t>General Studies B.G.S., WITH Urban Studies Concentration</t>
+          <t>General Studies B.G.S., WITH urban studies concentration</t>
         </is>
       </c>
       <c r="B485" t="inlineStr">
@@ -33422,7 +33422,7 @@
     <row r="486">
       <c r="A486" t="inlineStr">
         <is>
-          <t>General Studies B.G.S., WITH Women'S, Gender, And Sexuality Studies Concentration</t>
+          <t>General Studies B.G.S., WITH Women's,  gender,  and sexuality studies concentration</t>
         </is>
       </c>
       <c r="B486" t="inlineStr">
@@ -33966,7 +33966,7 @@
     <row r="494">
       <c r="A494" t="inlineStr">
         <is>
-          <t>Integrated Public Relations And Advertising B.S., WITH Advertising Concentration</t>
+          <t>Integrated Public Relations And Advertising B.S., WITH advertising concentration</t>
         </is>
       </c>
       <c r="B494" t="inlineStr">
@@ -34034,7 +34034,7 @@
     <row r="495">
       <c r="A495" t="inlineStr">
         <is>
-          <t>Integrated Public Relations And Advertising B.S., WITH Public Relations Concentration</t>
+          <t>Integrated Public Relations And Advertising B.S., WITH public relations concentration</t>
         </is>
       </c>
       <c r="B495" t="inlineStr">
@@ -34102,7 +34102,7 @@
     <row r="496">
       <c r="A496" t="inlineStr">
         <is>
-          <t>Mass Communications B.A., WITH News And Content Creation Concentration</t>
+          <t>Mass Communications B.A., WITH news and content creation concentration</t>
         </is>
       </c>
       <c r="B496" t="inlineStr">
@@ -34170,7 +34170,7 @@
     <row r="497">
       <c r="A497" t="inlineStr">
         <is>
-          <t>Mass Communications B.A., WITH Video And Documentary Production Concentration</t>
+          <t>Mass Communications B.A., WITH video and documentary production concentration</t>
         </is>
       </c>
       <c r="B497" t="inlineStr">
@@ -34850,7 +34850,7 @@
     <row r="507">
       <c r="A507" t="inlineStr">
         <is>
-          <t>Chemistry B.A., WITH Biochemistry/Biotechnology Concentration</t>
+          <t>Chemistry B.A., WITH biochemistry/biotechnology concentration</t>
         </is>
       </c>
       <c r="B507" t="inlineStr">
@@ -35530,7 +35530,7 @@
     <row r="517">
       <c r="A517" t="inlineStr">
         <is>
-          <t>English B.A., WITH Creative Writing Concentration</t>
+          <t>English B.A., WITH creative writing concentration</t>
         </is>
       </c>
       <c r="B517" t="inlineStr">
@@ -35870,7 +35870,7 @@
     <row r="522">
       <c r="A522" t="inlineStr">
         <is>
-          <t>Environmental Science And Policy B.S., WITH Environmental Analysis Concentration</t>
+          <t>Environmental Science And Policy B.S., WITH environmental analysis concentration</t>
         </is>
       </c>
       <c r="B522" t="inlineStr">
@@ -35938,7 +35938,7 @@
     <row r="523">
       <c r="A523" t="inlineStr">
         <is>
-          <t>Environmental Science And Policy B.S., WITH Environmental Policy And Sustainability Concentration</t>
+          <t>Environmental Science And Policy B.S., WITH environmental policy and sustainability concentration</t>
         </is>
       </c>
       <c r="B523" t="inlineStr">
@@ -36006,7 +36006,7 @@
     <row r="524">
       <c r="A524" t="inlineStr">
         <is>
-          <t>Environmental Science And Policy B.S., WITH Environmental Science Concentration</t>
+          <t>Environmental Science And Policy B.S., WITH environmental science concentration</t>
         </is>
       </c>
       <c r="B524" t="inlineStr">
@@ -36074,7 +36074,7 @@
     <row r="525">
       <c r="A525" t="inlineStr">
         <is>
-          <t>Geography And Geographic Information Systems B.A., WITH Geographic Information Systems Concentration</t>
+          <t>Geography And Geographic Information Systems B.A., WITH geographic information systems concentration</t>
         </is>
       </c>
       <c r="B525" t="inlineStr">
@@ -36142,7 +36142,7 @@
     <row r="526">
       <c r="A526" t="inlineStr">
         <is>
-          <t>Geography And Geographic Information Systems B.A., WITH Geography Concentration</t>
+          <t>Geography And Geographic Information Systems B.A., WITH geography concentration</t>
         </is>
       </c>
       <c r="B526" t="inlineStr">
@@ -36210,7 +36210,7 @@
     <row r="527">
       <c r="A527" t="inlineStr">
         <is>
-          <t>Geography And Geographic Information Systems B.A., WITH Society And Environment Concentration</t>
+          <t>Geography And Geographic Information Systems B.A., WITH society and environment concentration</t>
         </is>
       </c>
       <c r="B527" t="inlineStr">
@@ -36752,7 +36752,7 @@
     <row r="535">
       <c r="A535" t="inlineStr">
         <is>
-          <t>Humanities And Cultural Studies B.A., WITH American Studies Concentration</t>
+          <t>Humanities And Cultural Studies B.A., WITH american studies concentration</t>
         </is>
       </c>
       <c r="B535" t="inlineStr">
@@ -36956,7 +36956,7 @@
     <row r="538">
       <c r="A538" t="inlineStr">
         <is>
-          <t>Information Science B.S., WITH Data Science And Analytics Concentration</t>
+          <t>Information Science B.S., WITH data science and analytics concentration</t>
         </is>
       </c>
       <c r="B538" t="inlineStr">
@@ -37024,7 +37024,7 @@
     <row r="539">
       <c r="A539" t="inlineStr">
         <is>
-          <t>Information Science B.S., WITH Health Informatics Concentration</t>
+          <t>Information Science B.S., WITH health informatics concentration</t>
         </is>
       </c>
       <c r="B539" t="inlineStr">
@@ -37092,7 +37092,7 @@
     <row r="540">
       <c r="A540" t="inlineStr">
         <is>
-          <t>Information Science B.S., WITH Information Security Concentration</t>
+          <t>Information Science B.S., WITH information security concentration</t>
         </is>
       </c>
       <c r="B540" t="inlineStr">
@@ -37160,7 +37160,7 @@
     <row r="541">
       <c r="A541" t="inlineStr">
         <is>
-          <t>Information Science B.S., WITH Intelligence Analysis Concentration</t>
+          <t>Information Science B.S., WITH intelligence analysis concentration</t>
         </is>
       </c>
       <c r="B541" t="inlineStr">
@@ -37228,7 +37228,7 @@
     <row r="542">
       <c r="A542" t="inlineStr">
         <is>
-          <t>Information Science B.S., WITH Web Development Technologies Concentration</t>
+          <t>Information Science B.S., WITH web development technologies concentration</t>
         </is>
       </c>
       <c r="B542" t="inlineStr">
@@ -37500,7 +37500,7 @@
     <row r="546">
       <c r="A546" t="inlineStr">
         <is>
-          <t>Biology B.S., WITH Animal Biology Concentration</t>
+          <t>Biology B.S., WITH animal biology concentration</t>
         </is>
       </c>
       <c r="B546" t="inlineStr">
@@ -37568,7 +37568,7 @@
     <row r="547">
       <c r="A547" t="inlineStr">
         <is>
-          <t>Biology B.S., WITH Ecology And Evolution Concentration</t>
+          <t>Biology B.S., WITH ecology and evolution concentration</t>
         </is>
       </c>
       <c r="B547" t="inlineStr">
@@ -37636,7 +37636,7 @@
     <row r="548">
       <c r="A548" t="inlineStr">
         <is>
-          <t>Biology B.S., WITH Medical Biology Concentration</t>
+          <t>Biology B.S., WITH medical biology concentration</t>
         </is>
       </c>
       <c r="B548" t="inlineStr">
@@ -37704,7 +37704,7 @@
     <row r="549">
       <c r="A549" t="inlineStr">
         <is>
-          <t>Biology B.S., WITH Plant Biology Concentration</t>
+          <t>Biology B.S., WITH plant biology concentration</t>
         </is>
       </c>
       <c r="B549" t="inlineStr">
@@ -38384,7 +38384,7 @@
     <row r="559">
       <c r="A559" t="inlineStr">
         <is>
-          <t>Mathematics B.A., WITH Applied/Computational Mathematics Concentration</t>
+          <t>Mathematics B.A., WITH applied/computational mathematics concentration</t>
         </is>
       </c>
       <c r="B559" t="inlineStr">
@@ -38452,7 +38452,7 @@
     <row r="560">
       <c r="A560" t="inlineStr">
         <is>
-          <t>Mathematics B.A., WITH General Mathematics Concentration</t>
+          <t>Mathematics B.A., WITH general mathematics concentration</t>
         </is>
       </c>
       <c r="B560" t="inlineStr">
@@ -38520,7 +38520,7 @@
     <row r="561">
       <c r="A561" t="inlineStr">
         <is>
-          <t>Mathematics B.A., WITH Pure Mathematics Concentration</t>
+          <t>Mathematics B.A., WITH pure mathematics concentration</t>
         </is>
       </c>
       <c r="B561" t="inlineStr">
@@ -38588,7 +38588,7 @@
     <row r="562">
       <c r="A562" t="inlineStr">
         <is>
-          <t>Mathematics: Computational And Applied B.S., WITH Data Analytics And Business Intelligence Concentration</t>
+          <t>Mathematics: Computational And Applied B.S., WITH data analytics and business intelligence concentration</t>
         </is>
       </c>
       <c r="B562" t="inlineStr">
@@ -38656,7 +38656,7 @@
     <row r="563">
       <c r="A563" t="inlineStr">
         <is>
-          <t>Mathematics: Computational And Applied B.S., WITH Discrete Mathematics And Cryptography Concentration</t>
+          <t>Mathematics: Computational And Applied B.S., WITH discrete mathematics and cryptography concentration</t>
         </is>
       </c>
       <c r="B563" t="inlineStr">
@@ -39540,7 +39540,7 @@
     <row r="576">
       <c r="A576" t="inlineStr">
         <is>
-          <t>Psychology B.A., WITH Advanced Research Experience In Psychology Concentration</t>
+          <t>Psychology B.A., WITH advanced research experience in psychology concentration</t>
         </is>
       </c>
       <c r="B576" t="inlineStr">
@@ -39608,7 +39608,7 @@
     <row r="577">
       <c r="A577" t="inlineStr">
         <is>
-          <t>Psychology B.A., WITH Diversity Concentration</t>
+          <t>Psychology B.A., WITH diversity concentration</t>
         </is>
       </c>
       <c r="B577" t="inlineStr">
@@ -40084,7 +40084,7 @@
     <row r="584">
       <c r="A584" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH Africana Studies Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH africana studies concentration</t>
         </is>
       </c>
       <c r="B584" t="inlineStr">
@@ -40152,7 +40152,7 @@
     <row r="585">
       <c r="A585" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH Aging Sciences Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH aging sciences concentration</t>
         </is>
       </c>
       <c r="B585" t="inlineStr">
@@ -40220,7 +40220,7 @@
     <row r="586">
       <c r="A586" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH American Studies Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH american studies concentration</t>
         </is>
       </c>
       <c r="B586" t="inlineStr">
@@ -40288,7 +40288,7 @@
     <row r="587">
       <c r="A587" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH Anthropology Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH anthropology concentration</t>
         </is>
       </c>
       <c r="B587" t="inlineStr">
@@ -40356,7 +40356,7 @@
     <row r="588">
       <c r="A588" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH Behavioral Healthcare Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH behavioral healthcare concentration</t>
         </is>
       </c>
       <c r="B588" t="inlineStr">
@@ -40424,7 +40424,7 @@
     <row r="589">
       <c r="A589" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH Communication Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH communication concentration</t>
         </is>
       </c>
       <c r="B589" t="inlineStr">
@@ -40492,7 +40492,7 @@
     <row r="590">
       <c r="A590" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH Communication Sciences And Disorders Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH communication sciences and disorders concentration</t>
         </is>
       </c>
       <c r="B590" t="inlineStr">
@@ -40560,7 +40560,7 @@
     <row r="591">
       <c r="A591" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH Criminology Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH criminology concentration</t>
         </is>
       </c>
       <c r="B591" t="inlineStr">
@@ -40628,7 +40628,7 @@
     <row r="592">
       <c r="A592" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH Deaf Studies Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH deaf studies concentration</t>
         </is>
       </c>
       <c r="B592" t="inlineStr">
@@ -40696,7 +40696,7 @@
     <row r="593">
       <c r="A593" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH Economics Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH economics concentration</t>
         </is>
       </c>
       <c r="B593" t="inlineStr">
@@ -40764,7 +40764,7 @@
     <row r="594">
       <c r="A594" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH Environmental Science And Policy Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH environmental science and policy concentration</t>
         </is>
       </c>
       <c r="B594" t="inlineStr">
@@ -40832,7 +40832,7 @@
     <row r="595">
       <c r="A595" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH Geography Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH geography concentration</t>
         </is>
       </c>
       <c r="B595" t="inlineStr">
@@ -40900,7 +40900,7 @@
     <row r="596">
       <c r="A596" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH Government And Global Affairs Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH government and global affairs concentration</t>
         </is>
       </c>
       <c r="B596" t="inlineStr">
@@ -40968,7 +40968,7 @@
     <row r="597">
       <c r="A597" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH History Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH history concentration</t>
         </is>
       </c>
       <c r="B597" t="inlineStr">
@@ -41036,7 +41036,7 @@
     <row r="598">
       <c r="A598" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH Humanities Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH humanities concentration</t>
         </is>
       </c>
       <c r="B598" t="inlineStr">
@@ -41104,7 +41104,7 @@
     <row r="599">
       <c r="A599" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH Information Studies Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH information studies concentration</t>
         </is>
       </c>
       <c r="B599" t="inlineStr">
@@ -41172,7 +41172,7 @@
     <row r="600">
       <c r="A600" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH Integrated Community Research Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH integrated community research concentration</t>
         </is>
       </c>
       <c r="B600" t="inlineStr">
@@ -41240,7 +41240,7 @@
     <row r="601">
       <c r="A601" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH International Studies Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH international studies concentration</t>
         </is>
       </c>
       <c r="B601" t="inlineStr">
@@ -41308,7 +41308,7 @@
     <row r="602">
       <c r="A602" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH Latin American, Caribbean, And Latino Studies Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH latin american, Caribbean,  and latino studies concentration</t>
         </is>
       </c>
       <c r="B602" t="inlineStr">
@@ -41376,7 +41376,7 @@
     <row r="603">
       <c r="A603" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH Mass Communications Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH mass communications concentration</t>
         </is>
       </c>
       <c r="B603" t="inlineStr">
@@ -41444,7 +41444,7 @@
     <row r="604">
       <c r="A604" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH Political Science Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH political science concentration</t>
         </is>
       </c>
       <c r="B604" t="inlineStr">
@@ -41512,7 +41512,7 @@
     <row r="605">
       <c r="A605" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH Psychology Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH psychology concentration</t>
         </is>
       </c>
       <c r="B605" t="inlineStr">
@@ -41580,7 +41580,7 @@
     <row r="606">
       <c r="A606" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH Public Administration Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH public administration concentration</t>
         </is>
       </c>
       <c r="B606" t="inlineStr">
@@ -41648,7 +41648,7 @@
     <row r="607">
       <c r="A607" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH Public Health Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH public health concentration</t>
         </is>
       </c>
       <c r="B607" t="inlineStr">
@@ -41716,7 +41716,7 @@
     <row r="608">
       <c r="A608" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH Social Relations And Policy Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH social relations and policy concentration</t>
         </is>
       </c>
       <c r="B608" t="inlineStr">
@@ -41784,7 +41784,7 @@
     <row r="609">
       <c r="A609" t="inlineStr">
         <is>
-          <t>Interdisciplinary Social Sciences B.A., WITH Women'S And Gender Studies Concentration</t>
+          <t>Interdisciplinary Social Sciences B.A., WITH Women's and gender studies concentration</t>
         </is>
       </c>
       <c r="B609" t="inlineStr">
@@ -41920,7 +41920,7 @@
     <row r="611">
       <c r="A611" t="inlineStr">
         <is>
-          <t>Sociology B.A., WITH Identity And Community Concentration</t>
+          <t>Sociology B.A., WITH identity and community concentration</t>
         </is>
       </c>
       <c r="B611" t="inlineStr">
@@ -41988,7 +41988,7 @@
     <row r="612">
       <c r="A612" t="inlineStr">
         <is>
-          <t>Sociology B.A., WITH Inequality And Social Justice Concentration</t>
+          <t>Sociology B.A., WITH inequality and social justice concentration</t>
         </is>
       </c>
       <c r="B612" t="inlineStr">
@@ -42124,7 +42124,7 @@
     <row r="614">
       <c r="A614" t="inlineStr">
         <is>
-          <t>Women'S, GENDER, And Sexuality Studies B.A.</t>
+          <t>Women'S, GENDER, and sexuality studies b.a.</t>
         </is>
       </c>
       <c r="B614" t="inlineStr">
@@ -42260,7 +42260,7 @@
     <row r="616">
       <c r="A616" t="inlineStr">
         <is>
-          <t>Women'S, GENDER, And Sexuality Studies Minor</t>
+          <t>Women'S, GENDER, and sexuality studies minor</t>
         </is>
       </c>
       <c r="B616" t="inlineStr">
@@ -42328,7 +42328,7 @@
     <row r="617">
       <c r="A617" t="inlineStr">
         <is>
-          <t>World Languages And Cultures B.A., WITH Applied Linguistics Concentration</t>
+          <t>World Languages And Cultures B.A., WITH applied linguistics concentration</t>
         </is>
       </c>
       <c r="B617" t="inlineStr">
@@ -42396,7 +42396,7 @@
     <row r="618">
       <c r="A618" t="inlineStr">
         <is>
-          <t>World Languages And Cultures B.A., WITH Chinese Language And Culture Concentration</t>
+          <t>World Languages And Cultures B.A., WITH chinese language and culture concentration</t>
         </is>
       </c>
       <c r="B618" t="inlineStr">
@@ -42464,7 +42464,7 @@
     <row r="619">
       <c r="A619" t="inlineStr">
         <is>
-          <t>World Languages And Cultures B.A., WITH Classics Concentration</t>
+          <t>World Languages And Cultures B.A., WITH classics concentration</t>
         </is>
       </c>
       <c r="B619" t="inlineStr">
@@ -42532,7 +42532,7 @@
     <row r="620">
       <c r="A620" t="inlineStr">
         <is>
-          <t>World Languages And Cultures B.A., WITH East Asian Languages And Cultures Concentration</t>
+          <t>World Languages And Cultures B.A., WITH east asian languages and cultures concentration</t>
         </is>
       </c>
       <c r="B620" t="inlineStr">
@@ -42600,7 +42600,7 @@
     <row r="621">
       <c r="A621" t="inlineStr">
         <is>
-          <t>World Languages And Cultures B.A., WITH French And Francophone Studies Concentration</t>
+          <t>World Languages And Cultures B.A., WITH french and francophone studies concentration</t>
         </is>
       </c>
       <c r="B621" t="inlineStr">
@@ -42668,7 +42668,7 @@
     <row r="622">
       <c r="A622" t="inlineStr">
         <is>
-          <t>World Languages And Cultures B.A., WITH German Concentration</t>
+          <t>World Languages And Cultures B.A., WITH german concentration</t>
         </is>
       </c>
       <c r="B622" t="inlineStr">
@@ -42736,7 +42736,7 @@
     <row r="623">
       <c r="A623" t="inlineStr">
         <is>
-          <t>World Languages And Cultures B.A., WITH Interdisciplinary Classical Civilizations Concentration</t>
+          <t>World Languages And Cultures B.A., WITH interdisciplinary classical civilizations concentration</t>
         </is>
       </c>
       <c r="B623" t="inlineStr">
@@ -42804,7 +42804,7 @@
     <row r="624">
       <c r="A624" t="inlineStr">
         <is>
-          <t>World Languages And Cultures B.A., WITH Italian Concentration</t>
+          <t>World Languages And Cultures B.A., WITH italian concentration</t>
         </is>
       </c>
       <c r="B624" t="inlineStr">
@@ -42872,7 +42872,7 @@
     <row r="625">
       <c r="A625" t="inlineStr">
         <is>
-          <t>World Languages And Cultures B.A., WITH Russian Concentration</t>
+          <t>World Languages And Cultures B.A., WITH russian concentration</t>
         </is>
       </c>
       <c r="B625" t="inlineStr">
@@ -42940,7 +42940,7 @@
     <row r="626">
       <c r="A626" t="inlineStr">
         <is>
-          <t>World Languages And Cultures B.A., WITH Spanish And Latin American Studies Concentration</t>
+          <t>World Languages And Cultures B.A., WITH spanish and latin american studies concentration</t>
         </is>
       </c>
       <c r="B626" t="inlineStr">

</xml_diff>